<commit_message>
Changed the min function to max function for maximum total time acquired for processing
</commit_message>
<xml_diff>
--- a/results/TASK_MP.8.xlsx
+++ b/results/TASK_MP.8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nanodegrees\Sensor Fusion\CAMERA\2D_Feature_Matching_VS_CODE\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nanodegrees\Sensor Fusion\CAMERA\GITRepo_2dFeatureTracking\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64479040-1E99-4CB7-850C-159437D35009}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED449C8A-D60A-4576-AC5F-262564954E36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,8 +480,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,8 +700,8 @@
         <v>95</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>16.6296</v>
+        <f>MAX(F3:F11)</f>
+        <v>18.9343</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -891,8 +891,8 @@
         <v>115</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>16.752300000000002</v>
+        <f>MAX(F15:F23)</f>
+        <v>22.098800000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1082,8 +1082,8 @@
         <v>106</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>17.249300000000002</v>
+        <f>MAX(F27:F35)</f>
+        <v>22.247699999999998</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1273,8 +1273,8 @@
         <v>90</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>12.107799999999999</v>
+        <f>MAX(F39:F47)</f>
+        <v>18.195599999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1564,8 +1564,8 @@
         <v>112</v>
       </c>
       <c r="F72" s="5">
-        <f>MIN(F63:F71)</f>
-        <v>12.58</v>
+        <f>MAX(F63:F71)</f>
+        <v>16.934799999999999</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="F74" s="7">
         <f>MIN(F12,F24,F36,F48,F72)</f>
-        <v>12.107799999999999</v>
+        <v>16.934799999999999</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5473D962-0466-4BE9-960E-1F175331B2CD}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,8 +1814,8 @@
         <v>22</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>17.208400000000001</v>
+        <f>MAX(F3:F11)</f>
+        <v>40.023499999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2005,8 +2005,8 @@
         <v>28</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>17.1538</v>
+        <f>MAX(F15:F23)</f>
+        <v>39.058399999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2196,8 +2196,8 @@
         <v>25</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>16.970800000000001</v>
+        <f>MAX(F27:F35)</f>
+        <v>38.414700000000003</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2387,8 +2387,8 @@
         <v>21</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>12.401999999999999</v>
+        <f>MAX(F39:F47)</f>
+        <v>34.6355</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2678,8 +2678,8 @@
         <v>24</v>
       </c>
       <c r="F72" s="5">
-        <f>MIN(F63:F71)</f>
-        <v>16.738499999999998</v>
+        <f>MAX(F63:F71)</f>
+        <v>39.090200000000003</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="F74" s="7">
         <f>MIN(F12,F24,F36,F48,F72)</f>
-        <v>12.401999999999999</v>
+        <v>34.6355</v>
       </c>
     </row>
   </sheetData>
@@ -2704,8 +2704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CEB659-3777-4543-AB6D-1CF45266C44C}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2924,8 +2924,8 @@
         <v>256</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>6.3858899999999998</v>
+        <f>MAX(F3:F11)</f>
+        <v>7.1663500000000004</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3115,8 +3115,8 @@
         <v>332</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>6.2495900000000004</v>
+        <f>MAX(F15:F23)</f>
+        <v>8.1574899999999992</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3306,8 +3306,8 @@
         <v>323</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>6.3196899999999996</v>
+        <f>MAX(F27:F35)</f>
+        <v>8.5043000000000006</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3497,8 +3497,8 @@
         <v>265</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>6.4628199999999998</v>
+        <f>MAX(F39:F47)</f>
+        <v>7.1593099999999996</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3788,8 +3788,8 @@
         <v>326</v>
       </c>
       <c r="F72" s="5">
-        <f>MIN(F63:F71)</f>
-        <v>7.5461900000000002</v>
+        <f>MAX(F63:F71)</f>
+        <v>8.5992200000000008</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3802,7 +3802,7 @@
       </c>
       <c r="F74" s="7">
         <f>MIN(F12,F24,F36,F48,F72)</f>
-        <v>6.2495900000000004</v>
+        <v>7.1593099999999996</v>
       </c>
     </row>
   </sheetData>
@@ -3814,8 +3814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11723D8-9ADC-4D4F-B5FE-03E71DF7AB5E}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4034,8 +4034,8 @@
         <v>188</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>433.44600000000003</v>
+        <f>MAX(F3:F11)</f>
+        <v>439.66800000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4225,8 +4225,8 @@
         <v>207</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>438.05700000000002</v>
+        <f>MAX(F15:F23)</f>
+        <v>451.25900000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4416,8 +4416,8 @@
         <v>182</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>432.24099999999999</v>
+        <f>MAX(F27:F35)</f>
+        <v>441.24200000000002</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4607,8 +4607,8 @@
         <v>183</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>432.13900000000001</v>
+        <f>MAX(F39:F47)</f>
+        <v>442.92599999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -4898,8 +4898,8 @@
         <v>195</v>
       </c>
       <c r="F72" s="5">
-        <f>MIN(F63:F71)</f>
-        <v>432.80700000000002</v>
+        <f>MAX(F63:F71)</f>
+        <v>441.50700000000001</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="F74" s="7">
         <f>MIN(F12,F24,F36,F48,F72)</f>
-        <v>432.13900000000001</v>
+        <v>439.66800000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4924,8 +4924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB74795-C47E-4601-BCD7-374CBB989C06}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5144,8 +5144,8 @@
         <v>92</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>7.9926000000000004</v>
+        <f>MAX(F3:F11)</f>
+        <v>9.5858600000000003</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5335,8 +5335,8 @@
         <v>84</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>8.12852</v>
+        <f>MAX(F15:F23)</f>
+        <v>9.4787199999999991</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5526,8 +5526,8 @@
         <v>101</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>8.0960800000000006</v>
+        <f>MAX(F27:F35)</f>
+        <v>11.0725</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5717,8 +5717,8 @@
         <v>56</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>7.7959699999999996</v>
+        <f>MAX(F39:F47)</f>
+        <v>9.0332799999999995</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -6008,8 +6008,8 @@
         <v>95</v>
       </c>
       <c r="F72" s="5">
-        <f>MIN(F63:F71)</f>
-        <v>8.2188999999999997</v>
+        <f>MAX(F63:F71)</f>
+        <v>9.4231200000000008</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6022,7 +6022,7 @@
       </c>
       <c r="F74" s="7">
         <f>MIN(F12,F24,F36,F48,F72)</f>
-        <v>7.7959699999999996</v>
+        <v>9.0332799999999995</v>
       </c>
     </row>
   </sheetData>
@@ -6034,8 +6034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C6F1DC-0E4D-4033-BA63-BE6737DCA0DB}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6254,8 +6254,8 @@
         <v>146</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>110.21</v>
+        <f>MAX(F3:F11)</f>
+        <v>116.26300000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -6445,8 +6445,8 @@
         <v>152</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>112.652</v>
+        <f>MAX(F15:F23)</f>
+        <v>119.309</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -6636,8 +6636,8 @@
         <v>145</v>
       </c>
       <c r="F36" s="5">
-        <f>MIN(F27:F35)</f>
-        <v>114.998</v>
+        <f>MAX(F27:F35)</f>
+        <v>122.502</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -6827,8 +6827,8 @@
         <v>147</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>104.495</v>
+        <f>MAX(F39:F47)</f>
+        <v>117.401</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7018,8 +7018,8 @@
         <v>151</v>
       </c>
       <c r="F60" s="5">
-        <f>MIN(F51:F59)</f>
-        <v>108.236</v>
+        <f>MAX(F51:F59)</f>
+        <v>114.193</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7209,8 +7209,8 @@
         <v>154</v>
       </c>
       <c r="F73" s="5">
-        <f>MIN(F64:F72)</f>
-        <v>104.797</v>
+        <f>MAX(F64:F72)</f>
+        <v>112.36799999999999</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="F75" s="7">
         <f>MIN(F12,F24,F36,F48,F73)</f>
-        <v>104.495</v>
+        <v>112.36799999999999</v>
       </c>
     </row>
   </sheetData>
@@ -7235,8 +7235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82588046-DE93-4401-AEEB-2CE3A1EA0E06}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7455,8 +7455,8 @@
         <v>80</v>
       </c>
       <c r="F12" s="5">
-        <f>MIN(F3:F11)</f>
-        <v>128.91499999999999</v>
+        <f>MAX(F3:F11)</f>
+        <v>160.98400000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7646,8 +7646,8 @@
         <v>88</v>
       </c>
       <c r="F24" s="5">
-        <f>MIN(F15:F23)</f>
-        <v>156.26900000000001</v>
+        <f>MAX(F15:F23)</f>
+        <v>172.42500000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7941,8 +7941,8 @@
         <v>79</v>
       </c>
       <c r="F48" s="5">
-        <f>MIN(F39:F47)</f>
-        <v>155.96100000000001</v>
+        <f>MAX(F39:F47)</f>
+        <v>164.94499999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -8236,8 +8236,8 @@
         <v>104</v>
       </c>
       <c r="F73" s="5">
-        <f>MIN(F64:F72)</f>
-        <v>127.598</v>
+        <f>MAX(F64:F72)</f>
+        <v>150.75899999999999</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8250,7 +8250,7 @@
       </c>
       <c r="F75" s="7">
         <f>MIN(F12,F24,F36,F48,F73)</f>
-        <v>127.598</v>
+        <v>150.75899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>